<commit_message>
Added new fuel "Waste" to enable CHP_WasteToEnergy (only EE and NO for now); set FixedCosts and CapitalCosts for resource technologies to 0.01
</commit_message>
<xml_diff>
--- a/Conversion Script/Set_filter_file_Europe2060.xlsx
+++ b/Conversion Script/Set_filter_file_Europe2060.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\testbed\Documents\GENeSYS_MOD.data\Conversion Script\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nim\Documents\GENeSYS_MOD.data\Conversion Script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{81D135AD-9A63-467D-BAB5-DA91BB083ADD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B06E4F92-9222-4EB9-8BED-E37A287C0B9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="38616" windowHeight="21096" activeTab="3" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
   </bookViews>
   <sheets>
     <sheet name="Region_selection" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Storage_selection!$A$1:$B$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Technology_selection!$A$1:$B$154</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Technology_selection!$A$1:$B$156</definedName>
     <definedName name="Fuels">#REF!</definedName>
     <definedName name="Technologies">#REF!:B</definedName>
   </definedNames>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="295">
   <si>
     <t>DE</t>
   </si>
@@ -926,6 +926,15 @@
   </si>
   <si>
     <t>Heat_MediumHigh_Industrial</t>
+  </si>
+  <si>
+    <t>CHP_WasteToEnergy</t>
+  </si>
+  <si>
+    <t>R_Waste</t>
+  </si>
+  <si>
+    <t>Waste</t>
   </si>
 </sst>
 </file>
@@ -1291,16 +1300,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A667788-FC3C-4C43-9E46-ED47A2AEE749}">
   <dimension ref="A1:C55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>205</v>
       </c>
@@ -1309,7 +1318,7 @@
       </c>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>209</v>
       </c>
@@ -1318,7 +1327,7 @@
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1326,7 +1335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1334,7 +1343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1342,7 +1351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1350,7 +1359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1358,7 +1367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1366,7 +1375,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1374,7 +1383,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1382,7 +1391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1390,7 +1399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1398,7 +1407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -1406,7 +1415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1414,7 +1423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1422,7 +1431,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1430,7 +1439,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1438,7 +1447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1446,7 +1455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1454,7 +1463,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1462,7 +1471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1470,7 +1479,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1478,7 +1487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1486,7 +1495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1494,7 +1503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1502,7 +1511,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1510,7 +1519,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1518,7 +1527,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>1</v>
       </c>
@@ -1526,7 +1535,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -1534,7 +1543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -1542,7 +1551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -1550,7 +1559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -1558,7 +1567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -1566,7 +1575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -1574,7 +1583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -1582,7 +1591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -1590,7 +1599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -1598,7 +1607,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>210</v>
       </c>
@@ -1606,7 +1615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>211</v>
       </c>
@@ -1614,7 +1623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>212</v>
       </c>
@@ -1622,7 +1631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>213</v>
       </c>
@@ -1630,7 +1639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>214</v>
       </c>
@@ -1638,7 +1647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>215</v>
       </c>
@@ -1646,7 +1655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>216</v>
       </c>
@@ -1654,7 +1663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>217</v>
       </c>
@@ -1662,7 +1671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>218</v>
       </c>
@@ -1670,7 +1679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>219</v>
       </c>
@@ -1678,7 +1687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>220</v>
       </c>
@@ -1686,7 +1695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>221</v>
       </c>
@@ -1694,7 +1703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>222</v>
       </c>
@@ -1702,7 +1711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>223</v>
       </c>
@@ -1710,7 +1719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>224</v>
       </c>
@@ -1718,7 +1727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>225</v>
       </c>
@@ -1726,7 +1735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>226</v>
       </c>
@@ -1734,7 +1743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>227</v>
       </c>
@@ -1749,18 +1758,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C5D2E10-6D88-4A1E-9C1A-BD9E15FD6A9D}">
-  <dimension ref="A1:B154"/>
+  <dimension ref="A1:B156"/>
   <sheetViews>
-    <sheetView topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="F97" sqref="F97"/>
+    <sheetView topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="A136" sqref="A136"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>135</v>
       </c>
@@ -1768,7 +1777,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>37</v>
       </c>
@@ -1776,7 +1785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -1784,7 +1793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -1792,7 +1801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -1800,7 +1809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>41</v>
       </c>
@@ -1808,7 +1817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -1816,7 +1825,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>43</v>
       </c>
@@ -1824,7 +1833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>44</v>
       </c>
@@ -1832,7 +1841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>45</v>
       </c>
@@ -1840,7 +1849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>46</v>
       </c>
@@ -1848,7 +1857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>47</v>
       </c>
@@ -1856,7 +1865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>48</v>
       </c>
@@ -1864,7 +1873,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>49</v>
       </c>
@@ -1872,7 +1881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>50</v>
       </c>
@@ -1880,7 +1889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>51</v>
       </c>
@@ -1888,7 +1897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>52</v>
       </c>
@@ -1896,1110 +1905,1126 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>292</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>53</v>
       </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="B19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>54</v>
       </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="B20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>55</v>
       </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="B21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>56</v>
       </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="B22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>57</v>
       </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="B23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>279</v>
       </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="B24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>280</v>
       </c>
-      <c r="B24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="B25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>281</v>
       </c>
-      <c r="B25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="B26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>58</v>
       </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="B27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>59</v>
       </c>
-      <c r="B27">
+      <c r="B28">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+      <c r="B29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+      <c r="B30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+      <c r="B31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+      <c r="B32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+      <c r="B33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
+      <c r="B34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
+      <c r="B35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
+      <c r="B36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+      <c r="B37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
+      <c r="B38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="B39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>232</v>
       </c>
-      <c r="B39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="B40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
         <v>233</v>
       </c>
-      <c r="B40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="B41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
         <v>234</v>
       </c>
-      <c r="B41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="B42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
         <v>235</v>
       </c>
-      <c r="B42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="B43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
         <v>236</v>
       </c>
-      <c r="B43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="B44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
         <v>237</v>
       </c>
-      <c r="B44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="B45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
         <v>238</v>
       </c>
-      <c r="B45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="B46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
         <v>239</v>
       </c>
-      <c r="B46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="B47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
         <v>240</v>
       </c>
-      <c r="B47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="B48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
         <v>241</v>
       </c>
-      <c r="B48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+      <c r="B49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
         <v>242</v>
       </c>
-      <c r="B49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+      <c r="B50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
         <v>243</v>
       </c>
-      <c r="B50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+      <c r="B51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
         <v>285</v>
       </c>
-      <c r="B51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+      <c r="B52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
         <v>286</v>
       </c>
-      <c r="B52">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+      <c r="B53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
         <v>287</v>
       </c>
-      <c r="B53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+      <c r="B54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
         <v>288</v>
       </c>
-      <c r="B54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+      <c r="B55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
         <v>289</v>
       </c>
-      <c r="B55">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+      <c r="B56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
         <v>72</v>
       </c>
-      <c r="B56">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+      <c r="B57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
         <v>73</v>
       </c>
-      <c r="B57">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+      <c r="B58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
         <v>74</v>
       </c>
-      <c r="B58">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+      <c r="B59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
         <v>75</v>
       </c>
-      <c r="B59">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+      <c r="B60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
         <v>76</v>
       </c>
-      <c r="B60">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+      <c r="B61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
         <v>77</v>
       </c>
-      <c r="B61">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+      <c r="B62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
         <v>78</v>
       </c>
-      <c r="B62">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+      <c r="B63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
         <v>79</v>
       </c>
-      <c r="B63">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+      <c r="B64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
         <v>80</v>
       </c>
-      <c r="B64">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+      <c r="B65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
         <v>71</v>
       </c>
-      <c r="B65">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+      <c r="B66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
         <v>81</v>
       </c>
-      <c r="B66">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+      <c r="B67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
         <v>82</v>
       </c>
-      <c r="B67">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+      <c r="B68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
         <v>83</v>
       </c>
-      <c r="B68">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+      <c r="B69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
         <v>84</v>
       </c>
-      <c r="B69">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+      <c r="B70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
         <v>85</v>
       </c>
-      <c r="B70">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+      <c r="B71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
         <v>86</v>
       </c>
-      <c r="B71">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+      <c r="B72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
         <v>87</v>
       </c>
-      <c r="B72">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
+      <c r="B73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
         <v>88</v>
       </c>
-      <c r="B73">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+      <c r="B74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
         <v>89</v>
       </c>
-      <c r="B74">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
+      <c r="B75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
         <v>269</v>
       </c>
-      <c r="B75">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
+      <c r="B76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
         <v>270</v>
       </c>
-      <c r="B76">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
+      <c r="B77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
         <v>271</v>
       </c>
-      <c r="B77">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
+      <c r="B78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
         <v>272</v>
       </c>
-      <c r="B78">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
+      <c r="B79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
         <v>273</v>
       </c>
-      <c r="B79">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
+      <c r="B80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
         <v>274</v>
       </c>
-      <c r="B80">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+      <c r="B81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
         <v>275</v>
       </c>
-      <c r="B81">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
+      <c r="B82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
         <v>276</v>
       </c>
-      <c r="B82">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
+      <c r="B83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
         <v>277</v>
       </c>
-      <c r="B83">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
+      <c r="B84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
         <v>90</v>
       </c>
-      <c r="B84">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
+      <c r="B85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
         <v>91</v>
       </c>
-      <c r="B85">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+      <c r="B86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
         <v>92</v>
       </c>
-      <c r="B86">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
+      <c r="B87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
         <v>93</v>
       </c>
-      <c r="B87">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
+      <c r="B88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
         <v>94</v>
       </c>
-      <c r="B88">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
+      <c r="B89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
         <v>95</v>
       </c>
-      <c r="B89">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
+      <c r="B90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
         <v>250</v>
       </c>
-      <c r="B90">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
+      <c r="B91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
         <v>96</v>
       </c>
-      <c r="B91">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
+      <c r="B92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
         <v>99</v>
       </c>
-      <c r="B92">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
+      <c r="B93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
         <v>97</v>
       </c>
-      <c r="B93">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
+      <c r="B94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
         <v>98</v>
       </c>
-      <c r="B94">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
+      <c r="B95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
         <v>251</v>
       </c>
-      <c r="B95">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
+      <c r="B96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
         <v>100</v>
       </c>
-      <c r="B96">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
+      <c r="B97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
         <v>266</v>
       </c>
-      <c r="B97">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
+      <c r="B98">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
         <v>267</v>
       </c>
-      <c r="B98">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
+      <c r="B99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
         <v>101</v>
       </c>
-      <c r="B99">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
+      <c r="B100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
         <v>252</v>
       </c>
-      <c r="B100">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
+      <c r="B101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
         <v>102</v>
       </c>
-      <c r="B101">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
+      <c r="B102">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
         <v>253</v>
       </c>
-      <c r="B102">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
+      <c r="B103">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
         <v>254</v>
       </c>
-      <c r="B103">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
+      <c r="B104">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
         <v>255</v>
       </c>
-      <c r="B104">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
+      <c r="B105">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
         <v>256</v>
       </c>
-      <c r="B105">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
+      <c r="B106">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
         <v>257</v>
       </c>
-      <c r="B106">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
+      <c r="B107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
         <v>258</v>
       </c>
-      <c r="B107">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
+      <c r="B108">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
         <v>259</v>
       </c>
-      <c r="B108">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
+      <c r="B109">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
         <v>260</v>
       </c>
-      <c r="B109">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
+      <c r="B110">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
         <v>261</v>
       </c>
-      <c r="B110">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
+      <c r="B111">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
         <v>262</v>
       </c>
-      <c r="B111">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
+      <c r="B112">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
         <v>263</v>
       </c>
-      <c r="B112">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
+      <c r="B113">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
         <v>264</v>
       </c>
-      <c r="B113">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" s="2" t="s">
+      <c r="B114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A115" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B114">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A115" s="2" t="s">
+      <c r="B115">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A116" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B115">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A116" s="2" t="s">
+      <c r="B116">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A117" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B116">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A117" s="2" t="s">
+      <c r="B117">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A118" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B117">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A118" s="2" t="s">
+      <c r="B118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A119" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B118">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A119" s="2" t="s">
+      <c r="B119">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A120" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B119">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" s="2" t="s">
+      <c r="B120">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A121" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B120">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121" s="2" t="s">
+      <c r="B121">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A122" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B121">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A122" s="2" t="s">
+      <c r="B122">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A123" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B122">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A123" s="2" t="s">
+      <c r="B123">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A124" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B123">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
+      <c r="B124">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
         <v>244</v>
       </c>
-      <c r="B124">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
+      <c r="B125">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
         <v>113</v>
       </c>
-      <c r="B125">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
+      <c r="B126">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
         <v>114</v>
       </c>
-      <c r="B126">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
+      <c r="B127">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
         <v>115</v>
       </c>
-      <c r="B127">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
+      <c r="B128">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
         <v>245</v>
       </c>
-      <c r="B128">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
+      <c r="B129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
         <v>116</v>
       </c>
-      <c r="B129">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
+      <c r="B130">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A131" t="s">
         <v>117</v>
       </c>
-      <c r="B130">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
+      <c r="B131">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
         <v>246</v>
       </c>
-      <c r="B131">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
+      <c r="B132">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
         <v>247</v>
       </c>
-      <c r="B132">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
+      <c r="B133">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
         <v>248</v>
       </c>
-      <c r="B133">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
+      <c r="B134">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
+        <v>293</v>
+      </c>
+      <c r="B135">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
         <v>249</v>
       </c>
-      <c r="B134">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
+      <c r="B136">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
         <v>228</v>
       </c>
-      <c r="B135">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
+      <c r="B137">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
         <v>231</v>
       </c>
-      <c r="B136">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
+      <c r="B138">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A139" t="s">
         <v>118</v>
       </c>
-      <c r="B137">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A138" s="2" t="s">
+      <c r="B139">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A140" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B138">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A139" s="2" t="s">
+      <c r="B140">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A141" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="B139">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
+      <c r="B141">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A142" t="s">
         <v>278</v>
       </c>
-      <c r="B140">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A141" s="2" t="s">
+      <c r="B142">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A143" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B141">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A142" s="2" t="s">
+      <c r="B143">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A144" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="B142">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
+      <c r="B144">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A145" t="s">
         <v>123</v>
       </c>
-      <c r="B143">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
+      <c r="B145">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
         <v>229</v>
       </c>
-      <c r="B144">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
+      <c r="B146">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A147" t="s">
         <v>124</v>
       </c>
-      <c r="B145">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
+      <c r="B147">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A148" t="s">
         <v>125</v>
       </c>
-      <c r="B146">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
+      <c r="B148">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A149" t="s">
         <v>230</v>
       </c>
-      <c r="B147">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
+      <c r="B149">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A150" t="s">
         <v>126</v>
       </c>
-      <c r="B148">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
+      <c r="B150">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A151" t="s">
         <v>127</v>
       </c>
-      <c r="B149">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A150" t="s">
+      <c r="B151">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A152" t="s">
         <v>128</v>
       </c>
-      <c r="B150">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A151" s="2" t="s">
+      <c r="B152">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A153" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B151">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A152" t="s">
+      <c r="B153">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A154" t="s">
         <v>130</v>
       </c>
-      <c r="B152">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
+      <c r="B154">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A155" t="s">
         <v>131</v>
       </c>
-      <c r="B153">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A154" t="s">
+      <c r="B155">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A156" t="s">
         <v>132</v>
       </c>
-      <c r="B154">
+      <c r="B156">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B154" xr:uid="{8C5D2E10-6D88-4A1E-9C1A-BD9E15FD6A9D}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B154">
-      <sortCondition ref="A1:A154"/>
+  <autoFilter ref="A1:B156" xr:uid="{8C5D2E10-6D88-4A1E-9C1A-BD9E15FD6A9D}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B156">
+      <sortCondition ref="A1:A156"/>
     </sortState>
   </autoFilter>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A68 A31:A34 A144 A16:A17" xr:uid="{F3A41512-0F1A-4AAA-A425-8857F9308381}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A69 A32:A35 A146 A16:A18" xr:uid="{F3A41512-0F1A-4AAA-A425-8857F9308381}">
       <formula1>Technologies</formula1>
     </dataValidation>
   </dataValidations>
@@ -3015,12 +3040,12 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>170</v>
       </c>
@@ -3028,7 +3053,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>173</v>
       </c>
@@ -3036,7 +3061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>174</v>
       </c>
@@ -3044,7 +3069,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>175</v>
       </c>
@@ -3052,7 +3077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>172</v>
       </c>
@@ -3060,7 +3085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>176</v>
       </c>
@@ -3068,7 +3093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>282</v>
       </c>
@@ -3076,7 +3101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>284</v>
       </c>
@@ -3084,7 +3109,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>283</v>
       </c>
@@ -3092,7 +3117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>171</v>
       </c>
@@ -3112,18 +3137,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C7942D6-5BBA-4326-BEB2-07D45E712A14}">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>138</v>
       </c>
@@ -3131,7 +3156,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>162</v>
       </c>
@@ -3139,7 +3164,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>139</v>
       </c>
@@ -3147,7 +3172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>140</v>
       </c>
@@ -3155,7 +3180,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>156</v>
       </c>
@@ -3163,7 +3188,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>141</v>
       </c>
@@ -3171,7 +3196,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>163</v>
       </c>
@@ -3179,7 +3204,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>164</v>
       </c>
@@ -3187,7 +3212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>165</v>
       </c>
@@ -3195,7 +3220,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>151</v>
       </c>
@@ -3203,7 +3228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>144</v>
       </c>
@@ -3211,7 +3236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>152</v>
       </c>
@@ -3219,7 +3244,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>143</v>
       </c>
@@ -3227,7 +3252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>268</v>
       </c>
@@ -3235,7 +3260,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>142</v>
       </c>
@@ -3243,7 +3268,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>265</v>
       </c>
@@ -3251,7 +3276,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>166</v>
       </c>
@@ -3259,7 +3284,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>155</v>
       </c>
@@ -3267,7 +3292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>153</v>
       </c>
@@ -3275,7 +3300,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>154</v>
       </c>
@@ -3283,7 +3308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>290</v>
       </c>
@@ -3291,7 +3316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>291</v>
       </c>
@@ -3299,7 +3324,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>159</v>
       </c>
@@ -3307,7 +3332,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>161</v>
       </c>
@@ -3315,7 +3340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>150</v>
       </c>
@@ -3323,7 +3348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>158</v>
       </c>
@@ -3331,7 +3356,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>160</v>
       </c>
@@ -3339,7 +3364,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>148</v>
       </c>
@@ -3347,7 +3372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>149</v>
       </c>
@@ -3355,7 +3380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>145</v>
       </c>
@@ -3363,7 +3388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>146</v>
       </c>
@@ -3371,7 +3396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>147</v>
       </c>
@@ -3379,7 +3404,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>157</v>
       </c>
@@ -3387,11 +3412,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>157</v>
       </c>
       <c r="B34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>294</v>
+      </c>
+      <c r="B35">
         <v>1</v>
       </c>
     </row>
@@ -3419,9 +3452,9 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>168</v>
       </c>
@@ -3429,7 +3462,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3437,7 +3470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3445,7 +3478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3453,7 +3486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3461,7 +3494,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3469,7 +3502,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3490,9 +3523,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>133</v>
       </c>
@@ -3500,7 +3533,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>134</v>
       </c>
@@ -3521,9 +3554,9 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>208</v>
       </c>
@@ -3531,7 +3564,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>178</v>
       </c>
@@ -3539,7 +3572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>179</v>
       </c>
@@ -3547,7 +3580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>180</v>
       </c>
@@ -3555,7 +3588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>181</v>
       </c>
@@ -3563,7 +3596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>182</v>
       </c>
@@ -3571,7 +3604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>183</v>
       </c>
@@ -3579,7 +3612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>184</v>
       </c>
@@ -3587,7 +3620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>185</v>
       </c>
@@ -3595,7 +3628,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>186</v>
       </c>
@@ -3603,7 +3636,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>187</v>
       </c>
@@ -3611,7 +3644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>188</v>
       </c>
@@ -3619,7 +3652,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>189</v>
       </c>
@@ -3627,7 +3660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>190</v>
       </c>
@@ -3635,7 +3668,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>191</v>
       </c>
@@ -3643,7 +3676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>192</v>
       </c>
@@ -3651,7 +3684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>193</v>
       </c>
@@ -3659,7 +3692,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>194</v>
       </c>
@@ -3667,7 +3700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>195</v>
       </c>
@@ -3688,9 +3721,9 @@
       <selection activeCell="Q37" sqref="Q37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>207</v>
       </c>
@@ -3698,7 +3731,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>147</v>
       </c>
@@ -3706,7 +3739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>197</v>
       </c>
@@ -3714,7 +3747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>198</v>
       </c>
@@ -3722,7 +3755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>199</v>
       </c>
@@ -3730,7 +3763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>200</v>
       </c>
@@ -3738,7 +3771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>201</v>
       </c>
@@ -3746,7 +3779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>202</v>
       </c>
@@ -3754,7 +3787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>203</v>
       </c>
@@ -3775,9 +3808,9 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>206</v>
       </c>
@@ -3786,7 +3819,7 @@
       </c>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2015</v>
       </c>
@@ -3794,7 +3827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2018</v>
       </c>
@@ -3802,7 +3835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2019</v>
       </c>
@@ -3810,7 +3843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2020</v>
       </c>
@@ -3818,7 +3851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2021</v>
       </c>
@@ -3826,7 +3859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2025</v>
       </c>
@@ -3834,7 +3867,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2030</v>
       </c>
@@ -3842,7 +3875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2035</v>
       </c>
@@ -3850,7 +3883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2040</v>
       </c>
@@ -3858,7 +3891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2045</v>
       </c>
@@ -3866,7 +3899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2050</v>
       </c>
@@ -3874,7 +3907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2055</v>
       </c>
@@ -3882,7 +3915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2060</v>
       </c>

</xml_diff>